<commit_message>
start of membership can accept today's date
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/membership.xlsx
+++ b/xforms/xlsforms/membership.xlsx
@@ -198,9 +198,6 @@
     <t>Start date of membership</t>
   </si>
   <si>
-    <t>. &lt; today()</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>processed</t>
+  </si>
+  <si>
+    <t>. &lt;= today()</t>
   </si>
 </sst>
 </file>
@@ -1393,7 +1393,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1629,7 +1629,7 @@
         <v>59</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I9" s="5" t="b">
         <v>1</v>
@@ -1638,16 +1638,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M10" s="5" t="b">
         <v>1</v>

</xml_diff>